<commit_message>
updated Correct page Title
</commit_message>
<xml_diff>
--- a/GuiTestAutomation/TestData/ProjectModule.xlsx
+++ b/GuiTestAutomation/TestData/ProjectModule.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GowriSoftSolutions\GuiTestAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\OnlineClasses\gowriSoftSolutions_Workspace\GUI_Framework\GuiTestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9159C04-6568-4AC5-AE32-542367B1F139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,9 +62,6 @@
     <t>TD_Description</t>
   </si>
   <si>
-    <t>Company1</t>
-  </si>
-  <si>
     <t>Project1</t>
   </si>
   <si>
@@ -85,12 +81,15 @@
   </si>
   <si>
     <t>2026#February#1#10#10</t>
+  </si>
+  <si>
+    <t>CTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,11 +432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
@@ -503,30 +502,30 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{D2453332-9806-4A4E-9D6B-8E15E7F8587B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"Chrome,Firefox"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>